<commit_message>
windows iRave problem and excell update
</commit_message>
<xml_diff>
--- a/labs/lab13/excel.xlsx
+++ b/labs/lab13/excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\IPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\IST\2ano\IIPM\git\labs\lab13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22EAACDF-15B6-41D4-8654-BCE49A6B21BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DE1AE4-26EA-4308-B0BB-3346609959FF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>Tarefa 1:</t>
   </si>
@@ -106,7 +106,22 @@
     <t>27 anos</t>
   </si>
   <si>
-    <t>Cabelareira</t>
+    <t>63 anos</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>0-10</t>
+  </si>
+  <si>
+    <t>16 anos</t>
+  </si>
+  <si>
+    <t>14 anos</t>
+  </si>
+  <si>
+    <t>cabeleireiro</t>
   </si>
 </sst>
 </file>
@@ -426,6 +441,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -462,7 +478,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
@@ -745,15 +760,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:T47"/>
+  <dimension ref="B4:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +783,7 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="3:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -776,29 +791,29 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
     </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D6" s="31" t="s">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="30" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="15" t="s">
@@ -806,15 +821,15 @@
       </c>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D7" s="32"/>
-      <c r="E7" s="30"/>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D7" s="33"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="10"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="24"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="25"/>
       <c r="J7" s="16"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="24"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="25"/>
       <c r="N7" s="16"/>
       <c r="S7" t="s">
         <v>12</v>
@@ -823,7 +838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>1</v>
       </c>
@@ -834,7 +849,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" s="17">
         <v>26.5</v>
@@ -843,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L8" s="17">
         <v>22.1</v>
@@ -852,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P8" t="s">
         <v>9</v>
@@ -870,7 +885,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
         <v>2</v>
       </c>
@@ -901,7 +916,7 @@
       <c r="N9" s="18">
         <v>5</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="Q9" t="s">
@@ -917,7 +932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" s="3">
         <v>3</v>
       </c>
@@ -964,7 +979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C11" s="3">
         <v>4</v>
       </c>
@@ -1011,7 +1026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C12" s="3">
         <v>5</v>
       </c>
@@ -1058,7 +1073,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C13" s="3">
         <v>6</v>
       </c>
@@ -1089,14 +1104,14 @@
       <c r="N13" s="18">
         <v>4</v>
       </c>
-      <c r="P13" s="35" t="s">
+      <c r="P13" s="23" t="s">
         <v>24</v>
       </c>
       <c r="Q13" t="s">
         <v>19</v>
       </c>
       <c r="R13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="S13" t="s">
         <v>17</v>
@@ -1105,47 +1120,155 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C14" s="3">
         <v>7</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="11"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D14" s="5">
+        <v>28</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
+        <v>3</v>
+      </c>
+      <c r="H14" s="17">
+        <v>47</v>
+      </c>
+      <c r="I14" s="17">
+        <v>2</v>
+      </c>
+      <c r="J14" s="18">
+        <v>4</v>
+      </c>
+      <c r="L14" s="17">
+        <v>60</v>
+      </c>
+      <c r="M14" s="17">
+        <v>1</v>
+      </c>
+      <c r="N14" s="18">
+        <v>5</v>
+      </c>
+      <c r="P14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>4</v>
+      </c>
+      <c r="U14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
         <v>8</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="11"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="18"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D15" s="5">
+        <v>11</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>6</v>
+      </c>
+      <c r="H15" s="17">
+        <v>22</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <v>6</v>
+      </c>
+      <c r="L15" s="17">
+        <v>45</v>
+      </c>
+      <c r="M15" s="17">
+        <v>2</v>
+      </c>
+      <c r="N15" s="18">
+        <v>4</v>
+      </c>
+      <c r="P15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R15" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
+      </c>
+      <c r="U15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
         <v>9</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="11"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="18"/>
+      <c r="D16" s="5">
+        <v>17</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
+        <v>5</v>
+      </c>
+      <c r="H16" s="17">
+        <v>59</v>
+      </c>
+      <c r="I16" s="17">
+        <v>4</v>
+      </c>
+      <c r="J16" s="18">
+        <v>4</v>
+      </c>
+      <c r="L16" s="17">
+        <v>43</v>
+      </c>
+      <c r="M16" s="17">
+        <v>0</v>
+      </c>
+      <c r="N16" s="18">
+        <v>5</v>
+      </c>
+      <c r="P16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>8</v>
+      </c>
+      <c r="U16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="3">
@@ -1451,45 +1574,45 @@
       <c r="N38" s="14"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="25"/>
+      <c r="C39" s="26"/>
       <c r="D39">
         <f>AVERAGE(D8:D37)</f>
-        <v>19.291666666666668</v>
+        <v>19.083333333333332</v>
       </c>
       <c r="E39">
         <f>AVERAGE(E8:E37)</f>
-        <v>0.33333333333333331</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F39">
         <f>AVERAGE(F8:F37)</f>
-        <v>3.8333333333333335</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="H39">
         <f>AVERAGE(H8:H37)</f>
-        <v>41.25</v>
+        <v>41.722222222222221</v>
       </c>
       <c r="I39">
         <f>AVERAGE(I8:I37)</f>
-        <v>0.66666666666666663</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="J39">
         <f>AVERAGE(J8:J37)</f>
-        <v>3.8333333333333335</v>
+        <v>4.4444444444444446</v>
       </c>
       <c r="L39">
         <f>AVERAGE(L8:L37)</f>
-        <v>50.85</v>
+        <v>50.344444444444449</v>
       </c>
       <c r="M39">
         <f>AVERAGE(M8:M37)</f>
-        <v>0.66666666666666663</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="N39">
         <f>AVERAGE(N8:N37)</f>
-        <v>3.8333333333333335</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -1505,41 +1628,41 @@
       <c r="N41" s="14"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="27"/>
+      <c r="C42" s="28"/>
       <c r="D42" s="8">
         <f>_xlfn.STDEV.S(D8:D37)</f>
-        <v>2.6665364551542692</v>
+        <v>4.8088460154178359</v>
       </c>
       <c r="E42" s="8">
         <f>_xlfn.STDEV.S(E8:E37)</f>
-        <v>0.81649658092772603</v>
+        <v>0.72648315725677892</v>
       </c>
       <c r="F42" s="8">
         <f>_xlfn.STDEV.S(F8:F37)</f>
-        <v>0.98319208025017457</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="H42" s="8">
         <f>_xlfn.STDEV.S(H8:H37)</f>
-        <v>10.769168955866558</v>
+        <v>12.730649804485408</v>
       </c>
       <c r="I42" s="8">
         <f>_xlfn.STDEV.S(I8:I37)</f>
-        <v>0.81649658092772603</v>
+        <v>1.3642254619787417</v>
       </c>
       <c r="J42" s="8">
         <f>_xlfn.STDEV.S(J8:J37)</f>
-        <v>1.1690451944500118</v>
+        <v>0.88191710368819731</v>
       </c>
       <c r="L42" s="8">
         <f>_xlfn.STDEV.S(L8:L37)</f>
-        <v>14.290381380495056</v>
+        <v>12.23898597833079</v>
       </c>
       <c r="M42" s="8">
         <f>_xlfn.STDEV.S(M8:M37)</f>
-        <v>0.81649658092772603</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N42" s="14" t="e">
         <v>#DIV/0!</v>
@@ -1610,10 +1733,10 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="28"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="8" t="e">
         <f>D39-D45</f>
         <v>#NUM!</v>

</xml_diff>